<commit_message>
lol - the order of cases being reported changed while I was writing the code
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -421,7 +421,7 @@
         </is>
       </c>
       <c r="F2" s="2">
-        <v>43889</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="F3" s="2">
-        <v>43894</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="F4" s="2">
-        <v>43895</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="5">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="F5" s="2">
-        <v>43896</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="6">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="F6" s="2">
-        <v>43897</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="7">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="F7" s="2">
-        <v>43904</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="8">
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="F8" s="2">
-        <v>43905</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="9">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="F9" s="2">
-        <v>43905</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="10">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="F10" s="2">
-        <v>43907</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="11">
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="F11" s="2">
-        <v>43907</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="12">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="F12" s="2">
-        <v>43907</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="13">
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="F13" s="2">
-        <v>43907</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="14">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="F14" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="15">
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="F15" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="16">
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="F16" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="17">
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="F17" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="18">
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="F18" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="19">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="F19" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="20">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="F20" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="21">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="F21" s="2">
-        <v>43908</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="22">
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="F22" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="23">
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="F23" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="24">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="F24" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="25">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="F25" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="26">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="F26" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="27">
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F27" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="28">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="F28" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="29">
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="F29" s="2">
-        <v>43909</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="30">
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="F30" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="31">
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="F31" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="32">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="F32" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="33">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="F33" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="34">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="F34" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="35">
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="F35" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="36">
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="F36" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="37">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="F37" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="38">
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="F38" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="39">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="F39" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="40">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="F40" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="41">
@@ -1513,7 +1513,7 @@
         </is>
       </c>
       <c r="F41" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="42">
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="F42" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="43">
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F43" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="44">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="F44" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="45">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="F45" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="46">
@@ -1653,7 +1653,7 @@
         </is>
       </c>
       <c r="F46" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="47">
@@ -1681,7 +1681,7 @@
         </is>
       </c>
       <c r="F47" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="48">
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="F48" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="49">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="F49" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="50">
@@ -1765,7 +1765,7 @@
         </is>
       </c>
       <c r="F50" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="51">
@@ -1793,7 +1793,7 @@
         </is>
       </c>
       <c r="F51" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="52">
@@ -1821,7 +1821,7 @@
         </is>
       </c>
       <c r="F52" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="53">
@@ -1849,7 +1849,7 @@
         </is>
       </c>
       <c r="F53" s="2">
-        <v>43911</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="54">
@@ -1877,7 +1877,7 @@
         </is>
       </c>
       <c r="F54" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="55">
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="F55" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="56">
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="F56" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="57">
@@ -1961,7 +1961,7 @@
         </is>
       </c>
       <c r="F57" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="58">
@@ -1989,7 +1989,7 @@
         </is>
       </c>
       <c r="F58" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="59">
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="F59" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="60">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="F60" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="61">
@@ -2073,7 +2073,7 @@
         </is>
       </c>
       <c r="F61" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="62">
@@ -2101,7 +2101,7 @@
         </is>
       </c>
       <c r="F62" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="63">
@@ -2129,7 +2129,7 @@
         </is>
       </c>
       <c r="F63" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="64">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="F64" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="65">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="F65" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="66">
@@ -2213,7 +2213,7 @@
         </is>
       </c>
       <c r="F66" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="67">
@@ -2241,7 +2241,7 @@
         </is>
       </c>
       <c r="F67" s="2">
-        <v>43912</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="68">
@@ -2269,7 +2269,7 @@
         </is>
       </c>
       <c r="F68" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="69">
@@ -2297,7 +2297,7 @@
         </is>
       </c>
       <c r="F69" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="70">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="F70" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="71">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="F71" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="72">
@@ -2381,7 +2381,7 @@
         </is>
       </c>
       <c r="F72" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="73">
@@ -2409,7 +2409,7 @@
         </is>
       </c>
       <c r="F73" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="74">
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="F74" s="2">
-        <v>43913</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="75">
@@ -2465,7 +2465,7 @@
         </is>
       </c>
       <c r="F75" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="76">
@@ -2493,7 +2493,7 @@
         </is>
       </c>
       <c r="F76" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="77">
@@ -2521,7 +2521,7 @@
         </is>
       </c>
       <c r="F77" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="78">
@@ -2549,7 +2549,7 @@
         </is>
       </c>
       <c r="F78" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="79">
@@ -2577,7 +2577,7 @@
         </is>
       </c>
       <c r="F79" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="80">
@@ -2605,7 +2605,7 @@
         </is>
       </c>
       <c r="F80" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="81">
@@ -2633,7 +2633,7 @@
         </is>
       </c>
       <c r="F81" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="82">
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="F82" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="83">
@@ -2689,7 +2689,7 @@
         </is>
       </c>
       <c r="F83" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="84">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="F84" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="85">
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="F85" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="86">
@@ -2773,7 +2773,7 @@
         </is>
       </c>
       <c r="F86" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="87">
@@ -2801,7 +2801,7 @@
         </is>
       </c>
       <c r="F87" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="88">
@@ -2829,7 +2829,7 @@
         </is>
       </c>
       <c r="F88" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="89">
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="F89" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="90">
@@ -2885,7 +2885,7 @@
         </is>
       </c>
       <c r="F90" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="91">
@@ -2913,7 +2913,7 @@
         </is>
       </c>
       <c r="F91" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="92">
@@ -2941,7 +2941,7 @@
         </is>
       </c>
       <c r="F92" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="93">
@@ -2969,7 +2969,7 @@
         </is>
       </c>
       <c r="F93" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="94">
@@ -2997,7 +2997,7 @@
         </is>
       </c>
       <c r="F94" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="95">
@@ -3025,7 +3025,7 @@
         </is>
       </c>
       <c r="F95" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="96">
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="F96" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="97">
@@ -3081,7 +3081,7 @@
         </is>
       </c>
       <c r="F97" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="98">
@@ -3109,7 +3109,7 @@
         </is>
       </c>
       <c r="F98" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="99">
@@ -3137,7 +3137,7 @@
         </is>
       </c>
       <c r="F99" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="100">
@@ -3165,7 +3165,7 @@
         </is>
       </c>
       <c r="F100" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="101">
@@ -3193,7 +3193,7 @@
         </is>
       </c>
       <c r="F101" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="102">
@@ -3221,7 +3221,7 @@
         </is>
       </c>
       <c r="F102" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="103">
@@ -3249,7 +3249,7 @@
         </is>
       </c>
       <c r="F103" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="104">
@@ -3277,7 +3277,7 @@
         </is>
       </c>
       <c r="F104" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="105">
@@ -3305,7 +3305,7 @@
         </is>
       </c>
       <c r="F105" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="106">
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="F106" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="107">
@@ -3361,7 +3361,7 @@
         </is>
       </c>
       <c r="F107" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="108">
@@ -3389,7 +3389,7 @@
         </is>
       </c>
       <c r="F108" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="109">
@@ -3417,7 +3417,7 @@
         </is>
       </c>
       <c r="F109" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="110">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="F110" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="111">
@@ -3473,7 +3473,7 @@
         </is>
       </c>
       <c r="F111" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="112">
@@ -3501,7 +3501,7 @@
         </is>
       </c>
       <c r="F112" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="113">
@@ -3529,7 +3529,7 @@
         </is>
       </c>
       <c r="F113" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="114">
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="F114" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="115">
@@ -3585,7 +3585,7 @@
         </is>
       </c>
       <c r="F115" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="116">
@@ -3613,7 +3613,7 @@
         </is>
       </c>
       <c r="F116" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="117">
@@ -3641,7 +3641,7 @@
         </is>
       </c>
       <c r="F117" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="118">
@@ -3669,7 +3669,7 @@
         </is>
       </c>
       <c r="F118" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="119">
@@ -3697,7 +3697,7 @@
         </is>
       </c>
       <c r="F119" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="120">
@@ -3725,7 +3725,7 @@
         </is>
       </c>
       <c r="F120" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="121">
@@ -3753,7 +3753,7 @@
         </is>
       </c>
       <c r="F121" s="2">
-        <v>43914</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="122">
@@ -4397,7 +4397,7 @@
         </is>
       </c>
       <c r="F144" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="145">
@@ -4425,7 +4425,7 @@
         </is>
       </c>
       <c r="F145" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="146">
@@ -4453,7 +4453,7 @@
         </is>
       </c>
       <c r="F146" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="147">
@@ -4481,7 +4481,7 @@
         </is>
       </c>
       <c r="F147" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="148">
@@ -4509,7 +4509,7 @@
         </is>
       </c>
       <c r="F148" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="149">
@@ -4537,7 +4537,7 @@
         </is>
       </c>
       <c r="F149" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="150">
@@ -4565,7 +4565,7 @@
         </is>
       </c>
       <c r="F150" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="151">
@@ -4593,7 +4593,7 @@
         </is>
       </c>
       <c r="F151" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="152">
@@ -4621,7 +4621,7 @@
         </is>
       </c>
       <c r="F152" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="153">
@@ -4649,7 +4649,7 @@
         </is>
       </c>
       <c r="F153" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="154">
@@ -4677,7 +4677,7 @@
         </is>
       </c>
       <c r="F154" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="155">
@@ -4705,7 +4705,7 @@
         </is>
       </c>
       <c r="F155" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="156">
@@ -4733,7 +4733,7 @@
         </is>
       </c>
       <c r="F156" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="157">
@@ -4761,7 +4761,7 @@
         </is>
       </c>
       <c r="F157" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="158">
@@ -4789,7 +4789,7 @@
         </is>
       </c>
       <c r="F158" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="159">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="F159" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="160">
@@ -4845,7 +4845,7 @@
         </is>
       </c>
       <c r="F160" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="161">
@@ -4873,7 +4873,7 @@
         </is>
       </c>
       <c r="F161" s="2">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="162">
@@ -4901,7 +4901,7 @@
         </is>
       </c>
       <c r="F162" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="163">
@@ -4929,7 +4929,7 @@
         </is>
       </c>
       <c r="F163" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="164">
@@ -4957,7 +4957,7 @@
         </is>
       </c>
       <c r="F164" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="165">
@@ -4985,7 +4985,7 @@
         </is>
       </c>
       <c r="F165" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="166">
@@ -5013,7 +5013,7 @@
         </is>
       </c>
       <c r="F166" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="167">
@@ -5041,7 +5041,7 @@
         </is>
       </c>
       <c r="F167" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="168">
@@ -5069,7 +5069,7 @@
         </is>
       </c>
       <c r="F168" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="169">
@@ -5097,7 +5097,7 @@
         </is>
       </c>
       <c r="F169" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="170">
@@ -5125,7 +5125,7 @@
         </is>
       </c>
       <c r="F170" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="171">
@@ -5153,7 +5153,7 @@
         </is>
       </c>
       <c r="F171" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="172">
@@ -5181,7 +5181,7 @@
         </is>
       </c>
       <c r="F172" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="173">
@@ -5209,7 +5209,7 @@
         </is>
       </c>
       <c r="F173" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="174">
@@ -5237,7 +5237,7 @@
         </is>
       </c>
       <c r="F174" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="175">
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="F175" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="176">
@@ -5293,7 +5293,7 @@
         </is>
       </c>
       <c r="F176" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="177">
@@ -5321,7 +5321,7 @@
         </is>
       </c>
       <c r="F177" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="178">
@@ -5349,7 +5349,7 @@
         </is>
       </c>
       <c r="F178" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="179">
@@ -5377,7 +5377,7 @@
         </is>
       </c>
       <c r="F179" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="180">
@@ -5405,7 +5405,7 @@
         </is>
       </c>
       <c r="F180" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="181">
@@ -5433,7 +5433,7 @@
         </is>
       </c>
       <c r="F181" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="182">
@@ -5461,7 +5461,7 @@
         </is>
       </c>
       <c r="F182" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="183">
@@ -5489,7 +5489,7 @@
         </is>
       </c>
       <c r="F183" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="184">
@@ -5517,7 +5517,7 @@
         </is>
       </c>
       <c r="F184" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="185">
@@ -5545,7 +5545,7 @@
         </is>
       </c>
       <c r="F185" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="186">
@@ -5573,7 +5573,7 @@
         </is>
       </c>
       <c r="F186" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="187">
@@ -5601,7 +5601,7 @@
         </is>
       </c>
       <c r="F187" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="188">
@@ -5629,7 +5629,7 @@
         </is>
       </c>
       <c r="F188" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="189">
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="F189" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="190">
@@ -5685,7 +5685,7 @@
         </is>
       </c>
       <c r="F190" s="2">
-        <v>43915</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="191">
@@ -5713,7 +5713,7 @@
         </is>
       </c>
       <c r="F191" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="192">
@@ -5741,7 +5741,7 @@
         </is>
       </c>
       <c r="F192" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="193">
@@ -5769,7 +5769,7 @@
         </is>
       </c>
       <c r="F193" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="194">
@@ -5797,7 +5797,7 @@
         </is>
       </c>
       <c r="F194" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="195">
@@ -5825,7 +5825,7 @@
         </is>
       </c>
       <c r="F195" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="196">
@@ -5853,7 +5853,7 @@
         </is>
       </c>
       <c r="F196" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="197">
@@ -5881,7 +5881,7 @@
         </is>
       </c>
       <c r="F197" s="2">
-        <v>43916</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="198">
@@ -5909,7 +5909,7 @@
         </is>
       </c>
       <c r="F198" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="199">
@@ -5937,7 +5937,7 @@
         </is>
       </c>
       <c r="F199" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="200">
@@ -5966,7 +5966,7 @@
         </is>
       </c>
       <c r="F200" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="201">
@@ -5995,7 +5995,7 @@
         </is>
       </c>
       <c r="F201" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="202">
@@ -6024,7 +6024,7 @@
         </is>
       </c>
       <c r="F202" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="203">
@@ -6052,7 +6052,7 @@
         </is>
       </c>
       <c r="F203" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="204">
@@ -6080,7 +6080,7 @@
         </is>
       </c>
       <c r="F204" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="205">
@@ -6108,7 +6108,7 @@
         </is>
       </c>
       <c r="F205" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="206">
@@ -6136,7 +6136,7 @@
         </is>
       </c>
       <c r="F206" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="207">
@@ -6164,7 +6164,7 @@
         </is>
       </c>
       <c r="F207" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="208">
@@ -6192,7 +6192,7 @@
         </is>
       </c>
       <c r="F208" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="209">
@@ -6220,7 +6220,7 @@
         </is>
       </c>
       <c r="F209" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="210">
@@ -6248,7 +6248,7 @@
         </is>
       </c>
       <c r="F210" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="211">
@@ -6277,7 +6277,7 @@
         </is>
       </c>
       <c r="F211" s="2">
-        <v>43916</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="212">
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="F212" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="213">
@@ -6334,7 +6334,7 @@
         </is>
       </c>
       <c r="F213" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="214">
@@ -6362,7 +6362,7 @@
         </is>
       </c>
       <c r="F214" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="215">
@@ -6391,7 +6391,7 @@
         </is>
       </c>
       <c r="F215" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="216">
@@ -6420,7 +6420,7 @@
         </is>
       </c>
       <c r="F216" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="217">
@@ -6448,7 +6448,7 @@
         </is>
       </c>
       <c r="F217" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="218">
@@ -6476,7 +6476,7 @@
         </is>
       </c>
       <c r="F218" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="219">
@@ -6505,7 +6505,7 @@
         </is>
       </c>
       <c r="F219" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="220">
@@ -6537,7 +6537,7 @@
         </is>
       </c>
       <c r="F220" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="221">
@@ -6565,7 +6565,7 @@
         </is>
       </c>
       <c r="F221" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="222">
@@ -6593,7 +6593,7 @@
         </is>
       </c>
       <c r="F222" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="223">
@@ -6621,7 +6621,7 @@
         </is>
       </c>
       <c r="F223" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="224">
@@ -6649,7 +6649,7 @@
         </is>
       </c>
       <c r="F224" s="2">
-        <v>43916</v>
+        <v>43911</v>
       </c>
     </row>
     <row r="225">
@@ -6677,7 +6677,7 @@
         </is>
       </c>
       <c r="F225" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="226">
@@ -6705,7 +6705,7 @@
         </is>
       </c>
       <c r="F226" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="227">
@@ -6733,7 +6733,7 @@
         </is>
       </c>
       <c r="F227" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="228">
@@ -6761,7 +6761,7 @@
         </is>
       </c>
       <c r="F228" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="229">
@@ -6789,7 +6789,7 @@
         </is>
       </c>
       <c r="F229" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="230">
@@ -6817,7 +6817,7 @@
         </is>
       </c>
       <c r="F230" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="231">
@@ -6845,7 +6845,7 @@
         </is>
       </c>
       <c r="F231" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="232">
@@ -6873,7 +6873,7 @@
         </is>
       </c>
       <c r="F232" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="233">
@@ -6901,7 +6901,7 @@
         </is>
       </c>
       <c r="F233" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="234">
@@ -6930,7 +6930,7 @@
         </is>
       </c>
       <c r="F234" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="235">
@@ -6958,7 +6958,7 @@
         </is>
       </c>
       <c r="F235" s="2">
-        <v>43916</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="236">
@@ -6986,7 +6986,7 @@
         </is>
       </c>
       <c r="F236" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="237">
@@ -7015,7 +7015,7 @@
         </is>
       </c>
       <c r="F237" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="238">
@@ -7043,7 +7043,7 @@
         </is>
       </c>
       <c r="F238" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="239">
@@ -7071,7 +7071,7 @@
         </is>
       </c>
       <c r="F239" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="240">
@@ -7099,7 +7099,7 @@
         </is>
       </c>
       <c r="F240" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="241">
@@ -7127,7 +7127,7 @@
         </is>
       </c>
       <c r="F241" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="242">
@@ -7155,7 +7155,7 @@
         </is>
       </c>
       <c r="F242" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="243">
@@ -7183,7 +7183,7 @@
         </is>
       </c>
       <c r="F243" s="2">
-        <v>43916</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="244">
@@ -7211,7 +7211,7 @@
         </is>
       </c>
       <c r="F244" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="245">
@@ -7239,7 +7239,7 @@
         </is>
       </c>
       <c r="F245" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="246">
@@ -7267,7 +7267,7 @@
         </is>
       </c>
       <c r="F246" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="247">
@@ -7295,7 +7295,7 @@
         </is>
       </c>
       <c r="F247" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="248">
@@ -7323,7 +7323,7 @@
         </is>
       </c>
       <c r="F248" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="249">
@@ -7351,7 +7351,7 @@
         </is>
       </c>
       <c r="F249" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="250">
@@ -7379,7 +7379,7 @@
         </is>
       </c>
       <c r="F250" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="251">
@@ -7407,7 +7407,7 @@
         </is>
       </c>
       <c r="F251" s="2">
-        <v>43916</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="252">
@@ -7435,7 +7435,7 @@
         </is>
       </c>
       <c r="F252" s="2">
-        <v>43916</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="253">
@@ -7463,7 +7463,7 @@
         </is>
       </c>
       <c r="F253" s="2">
-        <v>43916</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="254">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="F254" s="2">
-        <v>43916</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="255">
@@ -7521,7 +7521,7 @@
         </is>
       </c>
       <c r="F255" s="2">
-        <v>43916</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="256">
@@ -7549,7 +7549,7 @@
         </is>
       </c>
       <c r="F256" s="2">
-        <v>43916</v>
+        <v>43905</v>
       </c>
     </row>
     <row r="257">
@@ -7577,7 +7577,7 @@
         </is>
       </c>
       <c r="F257" s="2">
-        <v>43916</v>
+        <v>43905</v>
       </c>
     </row>
     <row r="258">
@@ -7605,7 +7605,7 @@
         </is>
       </c>
       <c r="F258" s="2">
-        <v>43916</v>
+        <v>43904</v>
       </c>
     </row>
     <row r="259">
@@ -7633,7 +7633,7 @@
         </is>
       </c>
       <c r="F259" s="2">
-        <v>43916</v>
+        <v>43897</v>
       </c>
     </row>
     <row r="260">
@@ -7661,7 +7661,7 @@
         </is>
       </c>
       <c r="F260" s="2">
-        <v>43916</v>
+        <v>43896</v>
       </c>
     </row>
     <row r="261">
@@ -7689,7 +7689,7 @@
         </is>
       </c>
       <c r="F261" s="2">
-        <v>43916</v>
+        <v>43895</v>
       </c>
     </row>
     <row r="262">
@@ -7717,7 +7717,7 @@
         </is>
       </c>
       <c r="F262" s="2">
-        <v>43916</v>
+        <v>43894</v>
       </c>
     </row>
     <row r="263">
@@ -7745,7 +7745,7 @@
         </is>
       </c>
       <c r="F263" s="2">
-        <v>43916</v>
+        <v>43889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>